<commit_message>
update to python 3.13
</commit_message>
<xml_diff>
--- a/data/history.xlsx
+++ b/data/history.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1078"/>
+  <dimension ref="A1:B1079"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11215,6 +11215,16 @@
         <v>104</v>
       </c>
     </row>
+    <row r="1079">
+      <c r="A1079" s="1" t="inlineStr">
+        <is>
+          <t>25 July 2025</t>
+        </is>
+      </c>
+      <c r="B1079" t="n">
+        <v>218</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>